<commit_message>
Corrected quantity of 460mm profile from 2 to 4
</commit_message>
<xml_diff>
--- a/PL104300-cage-bom.xlsx
+++ b/PL104300-cage-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chris/root/files/projs/ender5pro/enclosure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E62AE5-8627-A54E-B8D0-8F5B96CAA62F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22446EE-B3C8-CF41-B225-95A1727C9B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51280" yWindow="460" windowWidth="43660" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="222">
   <si>
     <t>Item</t>
   </si>
@@ -402,9 +402,6 @@
   </si>
   <si>
     <t>Used-On</t>
-  </si>
-  <si>
-    <t>PG.L, PX.R</t>
   </si>
   <si>
     <t>DR.FL, DR.FR, DR.R</t>
@@ -2573,8 +2570,8 @@
   </sheetPr>
   <dimension ref="B1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2595,11 +2592,11 @@
     <row r="1" spans="2:11" ht="16" thickBot="1"/>
     <row r="2" spans="2:11" ht="18">
       <c r="B2" s="123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="124"/>
       <c r="D2" s="125" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E2" s="125"/>
       <c r="F2" s="126"/>
@@ -2608,66 +2605,66 @@
     </row>
     <row r="3" spans="2:11" ht="18">
       <c r="B3" s="129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="130"/>
       <c r="D3" s="127" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="127"/>
       <c r="F3" s="128"/>
     </row>
     <row r="4" spans="2:11" ht="18">
       <c r="B4" s="129" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" s="130"/>
       <c r="D4" s="131" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="131"/>
       <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:11" ht="18">
       <c r="B5" s="129" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="130"/>
       <c r="D5" s="131" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" s="131"/>
       <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:11" ht="18">
       <c r="B6" s="129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C6" s="130"/>
       <c r="D6" s="131" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="131"/>
       <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:11" ht="19" thickBot="1">
       <c r="B7" s="118" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C7" s="135"/>
       <c r="D7" s="133" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="133"/>
       <c r="F7" s="134"/>
     </row>
     <row r="8" spans="2:11" ht="16" thickBot="1">
       <c r="B8" s="118" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="119"/>
       <c r="D8" s="48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
@@ -2688,7 +2685,7 @@
     </row>
     <row r="11" spans="2:11" ht="19" thickBot="1">
       <c r="B11" s="120" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="121"/>
       <c r="D11" s="121"/>
@@ -2702,7 +2699,7 @@
     </row>
     <row r="12" spans="2:11" s="3" customFormat="1" ht="16" thickBot="1">
       <c r="B12" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>1</v>
@@ -2740,16 +2737,16 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>62</v>
@@ -2763,16 +2760,16 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>63</v>
@@ -2786,19 +2783,19 @@
         <v>1</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
@@ -2818,13 +2815,13 @@
         <v>48</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G16" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
@@ -2844,10 +2841,10 @@
         <v>48</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>61</v>
@@ -2867,10 +2864,10 @@
         <v>48</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>64</v>
@@ -2890,10 +2887,10 @@
         <v>48</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>60</v>
@@ -2914,7 +2911,7 @@
         <v>68</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="2:11" s="3" customFormat="1">
@@ -2932,7 +2929,7 @@
         <v>73</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="2:11" s="3" customFormat="1">
@@ -2950,7 +2947,7 @@
         <v>74</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="2:11">
@@ -2971,7 +2968,7 @@
     </row>
     <row r="27" spans="2:11" ht="16" thickBot="1">
       <c r="C27" s="114" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" s="115"/>
       <c r="E27" s="40"/>
@@ -3042,7 +3039,7 @@
     <row r="32" spans="2:11">
       <c r="B32" s="39"/>
       <c r="C32" s="116" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D32" s="117"/>
       <c r="E32" s="37"/>
@@ -3330,7 +3327,7 @@
   </sheetPr>
   <dimension ref="B1:J143"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -3349,11 +3346,11 @@
     <row r="1" spans="2:8" ht="16" thickBot="1"/>
     <row r="2" spans="2:8" ht="18">
       <c r="B2" s="123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="146"/>
       <c r="D2" s="139" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E2" s="125"/>
       <c r="F2" s="125"/>
@@ -3362,11 +3359,11 @@
     </row>
     <row r="3" spans="2:8" ht="18">
       <c r="B3" s="129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="145"/>
       <c r="D3" s="140" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="127"/>
       <c r="F3" s="127"/>
@@ -3375,11 +3372,11 @@
     </row>
     <row r="4" spans="2:8" ht="18">
       <c r="B4" s="129" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" s="145"/>
       <c r="D4" s="141" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="131"/>
       <c r="F4" s="131"/>
@@ -3388,11 +3385,11 @@
     </row>
     <row r="5" spans="2:8" ht="18">
       <c r="B5" s="129" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="145"/>
       <c r="D5" s="141" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" s="131"/>
       <c r="F5" s="131"/>
@@ -3401,11 +3398,11 @@
     </row>
     <row r="6" spans="2:8" ht="18">
       <c r="B6" s="129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C6" s="145"/>
       <c r="D6" s="141" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="131"/>
       <c r="F6" s="131"/>
@@ -3414,11 +3411,11 @@
     </row>
     <row r="7" spans="2:8" ht="19" thickBot="1">
       <c r="B7" s="118" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C7" s="119"/>
       <c r="D7" s="142" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="133"/>
       <c r="F7" s="133"/>
@@ -3427,11 +3424,11 @@
     </row>
     <row r="8" spans="2:8" ht="16" thickBot="1">
       <c r="B8" s="118" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="119"/>
       <c r="D8" s="143" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E8" s="144"/>
       <c r="F8" s="29"/>
@@ -3441,7 +3438,7 @@
     <row r="10" spans="2:8" ht="16" thickBot="1"/>
     <row r="11" spans="2:8" ht="19" thickBot="1">
       <c r="B11" s="136" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" s="137"/>
       <c r="D11" s="137"/>
@@ -3452,7 +3449,7 @@
     </row>
     <row r="12" spans="2:8" s="3" customFormat="1" ht="16" thickBot="1">
       <c r="B12" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>121</v>
@@ -3481,7 +3478,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>66</v>
@@ -3501,7 +3498,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>66</v>
@@ -3521,7 +3518,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>118</v>
@@ -3541,7 +3538,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>120</v>
@@ -3561,7 +3558,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>50</v>
@@ -3581,7 +3578,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>50</v>
@@ -3601,7 +3598,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>50</v>
@@ -3621,7 +3618,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>50</v>
@@ -3641,7 +3638,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>50</v>
@@ -3661,7 +3658,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>66</v>
@@ -3670,7 +3667,7 @@
         <v>79</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="2:10" s="3" customFormat="1">
@@ -3684,7 +3681,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>66</v>
@@ -3704,7 +3701,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>50</v>
@@ -3724,7 +3721,7 @@
         <v>20</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>50</v>
@@ -3744,7 +3741,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>50</v>
@@ -3764,7 +3761,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>50</v>
@@ -3784,7 +3781,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>50</v>
@@ -3810,7 +3807,7 @@
         <v>118</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="2:10" s="3" customFormat="1">
@@ -3830,7 +3827,7 @@
         <v>120</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="2:10" s="3" customFormat="1">
@@ -5084,8 +5081,8 @@
   </sheetPr>
   <dimension ref="B2:Q96"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5120,11 +5117,11 @@
     </row>
     <row r="3" spans="2:17" ht="18">
       <c r="B3" s="123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" s="146"/>
       <c r="D3" s="139" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E3" s="125"/>
       <c r="F3" s="125"/>
@@ -5137,11 +5134,11 @@
     </row>
     <row r="4" spans="2:17" ht="18">
       <c r="B4" s="129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" s="145"/>
       <c r="D4" s="140" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="127"/>
       <c r="F4" s="127"/>
@@ -5149,11 +5146,11 @@
     </row>
     <row r="5" spans="2:17" ht="18">
       <c r="B5" s="129" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="145"/>
       <c r="D5" s="141" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="131"/>
       <c r="F5" s="131"/>
@@ -5161,11 +5158,11 @@
     </row>
     <row r="6" spans="2:17" ht="18">
       <c r="B6" s="129" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="145"/>
       <c r="D6" s="141" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" s="131"/>
       <c r="F6" s="131"/>
@@ -5173,11 +5170,11 @@
     </row>
     <row r="7" spans="2:17" ht="18">
       <c r="B7" s="129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="145"/>
       <c r="D7" s="141" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" s="131"/>
       <c r="F7" s="131"/>
@@ -5185,11 +5182,11 @@
     </row>
     <row r="8" spans="2:17" ht="19" thickBot="1">
       <c r="B8" s="118" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C8" s="119"/>
       <c r="D8" s="142" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="133"/>
       <c r="F8" s="133"/>
@@ -5197,11 +5194,11 @@
     </row>
     <row r="9" spans="2:17" ht="16" thickBot="1">
       <c r="B9" s="118" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="119"/>
       <c r="D9" s="143" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="144"/>
       <c r="F9" s="29"/>
@@ -5229,7 +5226,7 @@
     </row>
     <row r="12" spans="2:17" ht="19" thickBot="1">
       <c r="B12" s="120" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C12" s="121"/>
       <c r="D12" s="121"/>
@@ -5243,11 +5240,11 @@
       <c r="L12" s="121"/>
       <c r="M12" s="108">
         <f>SUM(M14:M33)</f>
-        <v>25.289820000000002</v>
+        <v>25.639420000000005</v>
       </c>
       <c r="Q12" s="112">
         <f>SUM(Q14:Q33)</f>
-        <v>223.34</v>
+        <v>227.46</v>
       </c>
     </row>
     <row r="13" spans="2:17" s="3" customFormat="1" ht="16" thickBot="1">
@@ -5273,19 +5270,19 @@
         <v>9</v>
       </c>
       <c r="I13" s="110" t="s">
+        <v>207</v>
+      </c>
+      <c r="J13" s="110" t="s">
         <v>208</v>
       </c>
-      <c r="J13" s="110" t="s">
+      <c r="K13" s="110" t="s">
         <v>209</v>
       </c>
-      <c r="K13" s="110" t="s">
-        <v>210</v>
-      </c>
       <c r="L13" s="110" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M13" s="106" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="2:17" s="3" customFormat="1">
@@ -5302,10 +5299,10 @@
         <v>66</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>82</v>
@@ -5347,10 +5344,10 @@
         <v>66</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>106</v>
@@ -5383,19 +5380,19 @@
         <v>203</v>
       </c>
       <c r="C16" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>80</v>
@@ -5410,7 +5407,7 @@
       </c>
       <c r="M16" s="107">
         <f t="shared" si="0"/>
-        <v>0.34960000000000002</v>
+        <v>0.69920000000000004</v>
       </c>
       <c r="O16" s="3">
         <v>500</v>
@@ -5420,7 +5417,7 @@
       </c>
       <c r="Q16" s="113">
         <f t="shared" si="1"/>
-        <v>4.12</v>
+        <v>8.24</v>
       </c>
     </row>
     <row r="17" spans="2:17" s="3" customFormat="1">
@@ -5437,10 +5434,10 @@
         <v>66</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>104</v>
@@ -5476,16 +5473,16 @@
         <v>6</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>65</v>
@@ -5521,16 +5518,16 @@
         <v>6</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>81</v>
@@ -5566,16 +5563,16 @@
         <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>79</v>
@@ -5611,17 +5608,17 @@
         <v>12.36</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I21" s="111"/>
       <c r="J21" s="111"/>
@@ -5653,7 +5650,7 @@
         <v>118</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="7" t="s">
@@ -5701,7 +5698,7 @@
         <v>118</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="7" t="s">
@@ -5749,7 +5746,7 @@
         <v>118</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="7" t="s">
@@ -5791,13 +5788,13 @@
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="7" t="s">
@@ -5845,11 +5842,11 @@
         <v>118</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I26" s="111">
         <v>670</v>
@@ -5887,17 +5884,17 @@
         <v>180</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I27" s="111"/>
       <c r="J27" s="111"/>
@@ -5923,17 +5920,17 @@
         <v>180</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I28" s="111"/>
       <c r="J28" s="111"/>
@@ -5959,13 +5956,13 @@
         <v>180</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="7" t="s">
@@ -5995,13 +5992,13 @@
         <v>180</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="7" t="s">
@@ -6031,17 +6028,17 @@
         <v>48</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I31" s="111"/>
       <c r="J31" s="111"/>
@@ -6067,13 +6064,13 @@
         <v>48</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="7" t="s">
@@ -6103,16 +6100,16 @@
         <v>36</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F33" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="G33" s="16" t="s">
         <v>204</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>205</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>67</v>
@@ -6152,16 +6149,16 @@
         <v>12</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>68</v>
@@ -6528,6 +6525,12 @@
     <sortCondition ref="B14:B34"/>
   </sortState>
   <mergeCells count="15">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
     <mergeCell ref="B12:L12"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -6537,12 +6540,6 @@
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:G8"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="42" orientation="landscape" r:id="rId1"/>
@@ -7043,7 +7040,7 @@
         <v>120</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -7075,59 +7072,59 @@
     <row r="1" spans="2:9" ht="16" thickBot="1"/>
     <row r="2" spans="2:9">
       <c r="B2" s="59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F2" s="61" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G2" s="60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H2" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="62" t="s">
         <v>163</v>
-      </c>
-      <c r="I2" s="62" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="16" thickBot="1">
       <c r="B3" s="63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" s="65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G3" s="64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H3" s="65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3" s="66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="68">
         <v>7.9000000000000001E-2</v>
@@ -7139,7 +7136,7 @@
         <v>63</v>
       </c>
       <c r="F4" s="71" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G4" s="72">
         <v>8.5999999999999993E-2</v>
@@ -7153,7 +7150,7 @@
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="74" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="55">
         <v>0.11799999999999999</v>
@@ -7165,7 +7162,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G5" s="58">
         <v>0.112</v>
@@ -7179,7 +7176,7 @@
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="55">
         <v>0.13800000000000001</v>
@@ -7191,7 +7188,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" s="58">
         <v>0.13800000000000001</v>
@@ -7205,7 +7202,7 @@
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="74" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" s="55">
         <v>0.157</v>
@@ -7217,7 +7214,7 @@
         <v>36</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G7" s="58">
         <v>0.16400000000000001</v>
@@ -7231,7 +7228,7 @@
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C8" s="55">
         <v>0.19700000000000001</v>
@@ -7243,7 +7240,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G8" s="58">
         <v>0.19</v>
@@ -7257,7 +7254,7 @@
     </row>
     <row r="9" spans="2:9" ht="16" thickBot="1">
       <c r="B9" s="76" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C9" s="77">
         <v>0.23599999999999999</v>
@@ -7269,7 +7266,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G9" s="81">
         <v>0.25</v>
@@ -7283,7 +7280,7 @@
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C11" s="53"/>
       <c r="D11" s="53"/>
@@ -7293,7 +7290,7 @@
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C12" s="53"/>
       <c r="D12" s="53"/>
@@ -7303,7 +7300,7 @@
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="53"/>
@@ -7313,12 +7310,12 @@
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="52" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added assembly pictures and instructions
</commit_message>
<xml_diff>
--- a/PL104300-cage-bom.xlsx
+++ b/PL104300-cage-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chris/root/files/projs/ender5pro/enclosure/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/files/projs/enclosure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22446EE-B3C8-CF41-B225-95A1727C9B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01A5ABF-ECA9-C044-BF97-A1029E82DBA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="5100" windowWidth="25600" windowHeight="14580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -701,7 +701,7 @@
     <t>Gasket Seal for 670 x 570 glass panel</t>
   </si>
   <si>
-    <t>TE</t>
+    <t xml:space="preserve">PS.K </t>
   </si>
 </sst>
 </file>
@@ -2570,8 +2570,8 @@
   </sheetPr>
   <dimension ref="B1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3327,8 +3327,8 @@
   </sheetPr>
   <dimension ref="B1:J143"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5081,8 +5081,8 @@
   </sheetPr>
   <dimension ref="B2:Q96"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6525,12 +6525,6 @@
     <sortCondition ref="B14:B34"/>
   </sortState>
   <mergeCells count="15">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
     <mergeCell ref="B12:L12"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -6540,6 +6534,12 @@
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:G8"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="42" orientation="landscape" r:id="rId1"/>

</xml_diff>